<commit_message>
new results. 2021/04/20 19:45
</commit_message>
<xml_diff>
--- a/res/MPED/res.xlsx
+++ b/res/MPED/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\final_res\MPED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C24DA0-6B74-40B1-BA05-12B8361F910E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF5735C-697D-472A-964A-1AA33D94ABA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>people</t>
   </si>
@@ -158,8 +158,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -498,7 +498,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>0.34760000000000002</v>
       </c>
     </row>
@@ -506,7 +506,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>0.33100000000000002</v>
       </c>
     </row>
@@ -538,7 +538,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>0.33450000000000002</v>
       </c>
     </row>
@@ -554,7 +554,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0.37619999999999998</v>
       </c>
     </row>
@@ -562,7 +562,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>0.35949999999999999</v>
       </c>
     </row>
@@ -570,7 +570,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>0.35949999999999999</v>
       </c>
     </row>
@@ -578,7 +578,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>0.32740000000000002</v>
       </c>
     </row>
@@ -586,7 +586,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>0.3488</v>
       </c>
     </row>
@@ -594,7 +594,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="4">
         <v>0.3024</v>
       </c>
     </row>
@@ -602,7 +602,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>0.35120000000000001</v>
       </c>
     </row>
@@ -610,8 +610,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
-        <v>0.35</v>
+      <c r="B17" s="3">
+        <v>0.37140000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
@@ -619,7 +619,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.42020000000000002</v>
+        <v>0.42980000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
@@ -634,7 +634,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>0.36430000000000001</v>
       </c>
     </row>
@@ -650,7 +650,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>0.3619</v>
       </c>
     </row>
@@ -682,7 +682,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>0.33689999999999998</v>
       </c>
     </row>
@@ -690,7 +690,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="4">
         <v>0.32500000000000001</v>
       </c>
     </row>
@@ -698,7 +698,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>0.37980000000000003</v>
       </c>
     </row>
@@ -714,7 +714,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>0.37740000000000001</v>
       </c>
     </row>
@@ -722,8 +722,8 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
-        <v>0.31669999999999998</v>
+      <c r="B31" s="4">
+        <v>0.32019999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
@@ -732,7 +732,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.37798000000000004</v>
+        <v>0.37912999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/04/21 15:43
</commit_message>
<xml_diff>
--- a/res/MPED/res.xlsx
+++ b/res/MPED/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\final_res\MPED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF5735C-697D-472A-964A-1AA33D94ABA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B816FE2-B38C-4C0E-BB79-53CD27B1801B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>people</t>
   </si>
@@ -158,8 +158,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -498,7 +498,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.34760000000000002</v>
       </c>
     </row>
@@ -506,7 +506,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.33100000000000002</v>
       </c>
     </row>
@@ -538,7 +538,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>0.33450000000000002</v>
       </c>
     </row>
@@ -554,7 +554,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>0.37619999999999998</v>
       </c>
     </row>
@@ -562,7 +562,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>0.35949999999999999</v>
       </c>
     </row>
@@ -570,7 +570,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>0.35949999999999999</v>
       </c>
     </row>
@@ -578,7 +578,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>0.32740000000000002</v>
       </c>
     </row>
@@ -586,7 +586,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>0.3488</v>
       </c>
     </row>
@@ -594,7 +594,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.3024</v>
       </c>
     </row>
@@ -602,7 +602,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <v>0.35120000000000001</v>
       </c>
     </row>
@@ -610,7 +610,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>0.37140000000000001</v>
       </c>
     </row>
@@ -634,8 +634,8 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>0.36430000000000001</v>
+      <c r="B20" s="4">
+        <v>0.37619999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
@@ -650,7 +650,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>0.3619</v>
       </c>
     </row>
@@ -682,7 +682,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>0.33689999999999998</v>
       </c>
     </row>
@@ -690,7 +690,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>0.32500000000000001</v>
       </c>
     </row>
@@ -698,7 +698,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>0.37980000000000003</v>
       </c>
     </row>
@@ -714,7 +714,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="4">
         <v>0.37740000000000001</v>
       </c>
     </row>
@@ -722,7 +722,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>0.32019999999999998</v>
       </c>
     </row>
@@ -732,7 +732,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.37912999999999997</v>
+        <v>0.37952666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/05/30 14:50
</commit_message>
<xml_diff>
--- a/res/MPED/res.xlsx
+++ b/res/MPED/res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1603563-9503-234D-9BE1-287FA584C9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A48FA10-FBFA-8D4B-9176-E69B18BFAE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>0.37140000000000001</v>
+        <v>0.3952</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15">
@@ -631,7 +631,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.42980000000000002</v>
+        <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15">
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.38801333333333327</v>
+        <v>0.38927999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/06/03 10:32
</commit_message>
<xml_diff>
--- a/res/MPED/res.xlsx
+++ b/res/MPED/res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A48FA10-FBFA-8D4B-9176-E69B18BFAE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F00BF6F-568E-0E49-8073-DEC9DA9C821D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -727,7 +727,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.4012</v>
+        <v>0.40600000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15">
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.38927999999999996</v>
+        <v>0.38943999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/06/09 18:06
</commit_message>
<xml_diff>
--- a/res/MPED/res.xlsx
+++ b/res/MPED/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F00BF6F-568E-0E49-8073-DEC9DA9C821D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EE7805-DB8D-374C-A0E2-771D3DDB8CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -551,7 +551,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>0.33450000000000002</v>
+        <v>0.3417</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15">
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.38943999999999995</v>
+        <v>0.38968000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/06/10 23:30
</commit_message>
<xml_diff>
--- a/res/MPED/res.xlsx
+++ b/res/MPED/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EE7805-DB8D-374C-A0E2-771D3DDB8CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FAAA54-7418-1345-9F22-103434884387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -735,7 +735,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <v>0.3357</v>
+        <v>0.34050000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15">
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.38968000000000003</v>
+        <v>0.38984000000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/06/20 20:21
</commit_message>
<xml_diff>
--- a/res/MPED/res.xlsx
+++ b/res/MPED/res.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FAAA54-7418-1345-9F22-103434884387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E176161A-FCE0-1746-8C95-9DE5612C406C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -543,7 +543,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0.41789999999999999</v>
+        <v>0.43330000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15">
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.38984000000000008</v>
+        <v>0.39035333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/06/23 12:36
</commit_message>
<xml_diff>
--- a/res/MPED/res.xlsx
+++ b/res/MPED/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/MPED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E176161A-FCE0-1746-8C95-9DE5612C406C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A874389A-9860-DE45-ADBB-94466E7F0C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,7 +551,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>0.3417</v>
+        <v>0.34399999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15">
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" s="5">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.39035333333333339</v>
+        <v>0.39043</v>
       </c>
     </row>
   </sheetData>

</xml_diff>